<commit_message>
Adding transport prices and area density. This was needed in the context of an LCA project
</commit_message>
<xml_diff>
--- a/Input/LUCA Table.xlsx
+++ b/Input/LUCA Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicog\Desktop\Nicolò\GitHub\LUCA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicog\Desktop\Nicolò\GitHub\LUCA\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A16277-CF7E-4052-ADAC-AEEA1FF51F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9058CC1-0C58-4416-A33A-91A70EEEE813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33825" yWindow="4965" windowWidth="27525" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="624" windowWidth="19176" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>natural_gas</t>
   </si>
@@ -87,6 +87,69 @@
   </si>
   <si>
     <t>H2</t>
+  </si>
+  <si>
+    <t>GWP100</t>
+  </si>
+  <si>
+    <t>kg / kg</t>
+  </si>
+  <si>
+    <t>Surface density</t>
+  </si>
+  <si>
+    <t>Sden</t>
+  </si>
+  <si>
+    <t>kg / m**2</t>
+  </si>
+  <si>
+    <t>rail_trans</t>
+  </si>
+  <si>
+    <t>wate_trans</t>
+  </si>
+  <si>
+    <t>land_trans</t>
+  </si>
+  <si>
+    <t>sea_trans</t>
+  </si>
+  <si>
+    <t>Price per unit of distance and mass</t>
+  </si>
+  <si>
+    <t>prDM</t>
+  </si>
+  <si>
+    <t>EUR / tonnes / km</t>
+  </si>
+  <si>
+    <t>Transport, freight train {GLO}</t>
+  </si>
+  <si>
+    <t>Transport, freight, inland waterways, barge {GLO}</t>
+  </si>
+  <si>
+    <t>Transport, freight, light commercial vehicle {GLO}</t>
+  </si>
+  <si>
+    <t>Transport, freight, lorry, unspecified {GLO}</t>
+  </si>
+  <si>
+    <t>Transport, freight, sea, container ship {GLO}</t>
+  </si>
+  <si>
+    <t>Global Warming Potential 100</t>
+  </si>
+  <si>
+    <t>truck_trans</t>
+  </si>
+  <si>
+    <t>Powder coat, steel {GLO}</t>
+  </si>
+  <si>
+    <t>powder</t>
   </si>
 </sst>
 </file>
@@ -439,48 +502,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="3"/>
-    <col min="3" max="3" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>14</v>
       </c>
       <c r="E1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -497,7 +615,7 @@
         <v>141.69999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -514,7 +632,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -532,7 +650,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -547,6 +665,63 @@
         <v>0.55865921787709505</v>
       </c>
       <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>29.8</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>0.8</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
unit conversion of powder
</commit_message>
<xml_diff>
--- a/Input/LUCA Table.xlsx
+++ b/Input/LUCA Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicog\Desktop\Nicolò\GitHub\LUCA\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\eNextHub\LUCA\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9058CC1-0C58-4416-A33A-91A70EEEE813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0333AD20-2E7E-4C02-BB48-FE8F00478018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="624" windowWidth="19176" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,25 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={18195A07-DB70-4A5C-B794-35F8C121ACB1}</author>
+  </authors>
+  <commentList>
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{18195A07-DB70-4A5C-B794-35F8C121ACB1}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    60 micron thickness, 8000 kg/m3 densitity assumed for steel powder coating
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
@@ -146,10 +165,10 @@
     <t>truck_trans</t>
   </si>
   <si>
+    <t>powder</t>
+  </si>
+  <si>
     <t>Powder coat, steel {GLO}</t>
-  </si>
-  <si>
-    <t>powder</t>
   </si>
 </sst>
 </file>
@@ -237,6 +256,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Lorenzo Rinaldi" id="{DCC88CEA-0E29-4EDE-AE8B-1AEF6AEADEDC}" userId="S::lorenzo.rinaldi@enextgen.it::960c1595-8349-47cd-ad6a-ab02c21200f5" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -500,27 +525,36 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="K9" dT="2023-12-21T10:43:58.82" personId="{DCC88CEA-0E29-4EDE-AE8B-1AEF6AEADEDC}" id="{18195A07-DB70-4A5C-B794-35F8C121ACB1}">
+    <text xml:space="preserve">60 micron thickness, 8000 kg/m3 densitity assumed for steel powder coating
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="3"/>
-    <col min="3" max="3" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.3046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" style="3"/>
+    <col min="3" max="3" width="15.84375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="D1" t="s">
         <v>14</v>
       </c>
@@ -543,10 +577,10 @@
         <v>33</v>
       </c>
       <c r="K1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -554,25 +588,25 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="D3" t="s">
         <v>1</v>
       </c>
@@ -595,10 +629,10 @@
         <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -615,7 +649,7 @@
         <v>141.69999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -632,7 +666,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -650,7 +684,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -668,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -685,7 +719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -696,10 +730,10 @@
         <v>21</v>
       </c>
       <c r="K9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -727,5 +761,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating NG's LHV with value from MISE
</commit_message>
<xml_diff>
--- a/Input/LUCA Table.xlsx
+++ b/Input/LUCA Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\eNextHub\LUCA\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicog\Desktop\Nicolò\GitHub\LUCA\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBD78FE-0C8D-488F-8F49-CDC96E5AC2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EE279A-4F52-414F-982C-44AC442913B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,11 +39,20 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={B2318A00-3BCE-441A-8436-2CE958223374}</author>
     <author>tc={18195A07-DB70-4A5C-B794-35F8C121ACB1}</author>
     <author>tc={6927D7A9-CFCB-4FDA-93C2-C775E8FCF84E}</author>
   </authors>
   <commentList>
-    <comment ref="L9" authorId="0" shapeId="0" xr:uid="{18195A07-DB70-4A5C-B794-35F8C121ACB1}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{B2318A00-3BCE-441A-8436-2CE958223374}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Using 'Density' and 38.1 MJ/mc, the value used by MISE</t>
+      </text>
+    </comment>
+    <comment ref="L9" authorId="1" shapeId="0" xr:uid="{18195A07-DB70-4A5C-B794-35F8C121ACB1}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -52,7 +61,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="M9" authorId="1" shapeId="0" xr:uid="{6927D7A9-CFCB-4FDA-93C2-C775E8FCF84E}">
+    <comment ref="M9" authorId="2" shapeId="0" xr:uid="{6927D7A9-CFCB-4FDA-93C2-C775E8FCF84E}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -228,7 +237,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +259,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -332,6 +347,7 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Lorenzo Rinaldi" id="{DCC88CEA-0E29-4EDE-AE8B-1AEF6AEADEDC}" userId="S::lorenzo.rinaldi@enextgen.it::960c1595-8349-47cd-ad6a-ab02c21200f5" providerId="AD"/>
+  <person displayName="Nicolò Golinucci" id="{3ADF9C4A-1E09-4079-9F34-B331D1189868}" userId="S::nicolo.golinucci@enextgen.it::78589ceb-2175-461f-80ec-32eecf3e7ff4" providerId="AD"/>
 </personList>
 </file>
 
@@ -598,6 +614,9 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D4" dT="2023-12-29T09:48:04.07" personId="{3ADF9C4A-1E09-4079-9F34-B331D1189868}" id="{B2318A00-3BCE-441A-8436-2CE958223374}">
+    <text>Using 'Density' and 38.1 MJ/mc, the value used by MISE</text>
+  </threadedComment>
   <threadedComment ref="L9" dT="2023-12-21T10:43:58.82" personId="{DCC88CEA-0E29-4EDE-AE8B-1AEF6AEADEDC}" id="{18195A07-DB70-4A5C-B794-35F8C121ACB1}">
     <text xml:space="preserve">60 micron thickness, 8000 kg/m3 densitity assumed for steel powder coating
 </text>
@@ -614,30 +633,30 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="3"/>
-    <col min="3" max="3" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="3"/>
+    <col min="3" max="3" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="21.28515625" customWidth="1"/>
+    <col min="8" max="11" width="17.5546875" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="21.33203125" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" customWidth="1"/>
-    <col min="18" max="19" width="21.140625" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" customWidth="1"/>
+    <col min="18" max="19" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -690,7 +709,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -740,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>1</v>
       </c>
@@ -790,7 +809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -801,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>55.5</v>
+        <v>53.212290502793302</v>
       </c>
       <c r="E4">
         <v>141.69999999999999</v>
@@ -813,7 +832,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -836,7 +855,7 @@
         <v>0.71599999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -860,7 +879,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -886,7 +905,7 @@
         <v>0.55865921787709505</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -909,7 +928,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -938,7 +957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -979,7 +998,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>